<commit_message>
Add correct version of bug report file
</commit_message>
<xml_diff>
--- a/Виявлені баги.xlsx
+++ b/Виявлені баги.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\my-cypress-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\cypress\My-cypress-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E3DB06B-E254-4316-BE0B-713C03D582E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DC2B79-960A-4E49-96AD-6A91F27763C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8275A6FE-39B9-4D7A-B097-D35035BD4B14}"/>
   </bookViews>
@@ -68,10 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
-  <si>
-    <t>Додаток написаний російською мовою</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
   <si>
     <t>Preconditions:</t>
   </si>
@@ -85,21 +82,12 @@
     <t>Expected result:</t>
   </si>
   <si>
-    <t>Сертифікати додаються не за тим полем</t>
-  </si>
-  <si>
     <t>Steps to reproduce:</t>
   </si>
   <si>
     <t>Натиснути кнопку "Добавить"</t>
   </si>
   <si>
-    <t>Кнопка "Добавить" не працює</t>
-  </si>
-  <si>
-    <t>Новий сертифікат не з'являється:</t>
-  </si>
-  <si>
     <t>Description:</t>
   </si>
   <si>
@@ -121,22 +109,67 @@
     <t>2. Завантажений хоча б один сертифікат</t>
   </si>
   <si>
-    <t>Кнопка "Додати" розташована знизу, а не зверху, і має не такий дизайн</t>
-  </si>
-  <si>
     <t>Кнопка "Додати" розташована знизу і має синій колір</t>
   </si>
   <si>
     <t>Кнопка "Додати" має бути зверху і білого кольору</t>
   </si>
   <si>
-    <t>Відсутня кнопка  вибору сертифіката через стандартний діалог</t>
-  </si>
-  <si>
     <t>Можна додати сертифікат тільки перетаскуванням, а кнопка додати через стандартний діалог відсутня</t>
   </si>
   <si>
     <t>Повинна бути можливість вибору сертифіката через стандартний діалог</t>
+  </si>
+  <si>
+    <t>1. При завантаженні сертифікату з невідповідною структурою (Тестовий_платник_4_(Тест)-8101906)  система повністю втрачає свою працездатність</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> При завантаженні сертифікату з невідповідною структурою (Тестовий_платник_4_(Тест)-8101906) відображається повідомлення про помилку, а при оновленні сторінки втрачається можливість завантажувати нові сертифікати і переглядати раніше завантажені</t>
+  </si>
+  <si>
+    <t>Повинно відображатись повідомлення про помилку, є можливість завантажувати нові сертифікати, попередньо завантажені сертифікати відображаються коректно</t>
+  </si>
+  <si>
+    <t>2. Інтерфейс написаний російською мовою</t>
+  </si>
+  <si>
+    <t>3. Сертифікати додаються не з тим полем</t>
+  </si>
+  <si>
+    <t>4. Кнопка "Додати" розташована знизу, а не зверху, і має дизайн, що відрізняється від дизайну на ескізі</t>
+  </si>
+  <si>
+    <t>5. Відсутня кнопка  вибору сертифіката через стандартний діалог</t>
+  </si>
+  <si>
+    <t>6. У разі відсутності завантажених сертифікатів не відображається інформація про це</t>
+  </si>
+  <si>
+    <t>Немає повідомлення про відсутність завантажених сертифікатів</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. У списку завантажених сертифікатів обраний сертифікат підсвічується не так, як вказано у вимогах до застосунку </t>
+  </si>
+  <si>
+    <t>2. Не завантажено жодного сертифікату</t>
+  </si>
+  <si>
+    <t>1. Завантажити декілька сертифікатів</t>
+  </si>
+  <si>
+    <t>2. Вибрати хоча б один з них</t>
+  </si>
+  <si>
+    <t>8. Система дозволяє завантажувати однакові сертифікати</t>
+  </si>
+  <si>
+    <t>(це не є багом, а проопзиція щодо покращення роботи застосунку)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Завантажити декілька сертифікатів, серед яких будуть однакові</t>
+  </si>
+  <si>
+    <t>При завантаженні вже раніше доданих сертифікатів виводити  повідомлення про те, що сертифікат вже був завантажений, і не завантажувати його</t>
   </si>
 </sst>
 </file>
@@ -253,13 +286,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>228601</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>100678</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -297,13 +330,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>49525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>103</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -341,13 +374,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>90</xdr:row>
+      <xdr:row>112</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>45721</xdr:colOff>
-      <xdr:row>105</xdr:row>
+      <xdr:row>127</xdr:row>
       <xdr:rowOff>28229</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -385,13 +418,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>110</xdr:row>
+      <xdr:row>132</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>408900</xdr:colOff>
-      <xdr:row>128</xdr:row>
+      <xdr:row>150</xdr:row>
       <xdr:rowOff>136731</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -429,13 +462,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>141</xdr:row>
+      <xdr:row>163</xdr:row>
       <xdr:rowOff>167641</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>327660</xdr:colOff>
-      <xdr:row>154</xdr:row>
+      <xdr:row>176</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -473,13 +506,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>160</xdr:row>
+      <xdr:row>182</xdr:row>
       <xdr:rowOff>15239</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>335280</xdr:colOff>
-      <xdr:row>177</xdr:row>
+      <xdr:row>199</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -517,13 +550,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3914286</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>85486</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -561,13 +594,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>227948</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>159634</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -593,6 +626,314 @@
         <a:xfrm>
           <a:off x="0" y="3733800"/>
           <a:ext cx="5219048" cy="3085714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>396241</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Рисунок 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{291D5006-DFDC-9AAA-DAAA-8B7787E1F7DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4777741" y="1615440"/>
+          <a:ext cx="4610099" cy="1554480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Рисунок 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E43CC6D1-D866-19BB-00E4-2EC434840EB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1226820"/>
+          <a:ext cx="4541520" cy="1371600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>91441</xdr:colOff>
+      <xdr:row>218</xdr:row>
+      <xdr:rowOff>106681</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Рисунок 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0262005-A995-DA92-DF55-06E76373652C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="41475661"/>
+          <a:ext cx="4472940" cy="1569720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>221</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>45721</xdr:colOff>
+      <xdr:row>234</xdr:row>
+      <xdr:rowOff>68581</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Рисунок 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A4F305C-AE4D-D215-B2E2-0A36D4CBE7BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="43106341"/>
+          <a:ext cx="4427220" cy="2446020"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>247</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>256</xdr:row>
+      <xdr:rowOff>129541</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Рисунок 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02EF0A54-34B0-6FD1-73B0-543BC4591AD3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="47861221"/>
+          <a:ext cx="6309360" cy="1775460"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>260</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>272</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Рисунок 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8CDD266-27F8-F49F-2EC2-BCFA731FE430}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="50238661"/>
+          <a:ext cx="6263640" cy="2301239"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>285</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>294</xdr:row>
+      <xdr:rowOff>121921</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Рисунок 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB92FAF6-A3BC-A63A-D6F4-C1EA39338F91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="55229761"/>
+          <a:ext cx="6195059" cy="1767840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -990,10 +1331,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6149879E-C46B-4A7C-A389-D80138182DFF}">
-  <dimension ref="A1:A200"/>
+  <dimension ref="A1:A299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="F167" sqref="F167"/>
+    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
+      <selection activeCell="A240" sqref="A240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1003,172 +1344,187 @@
   <sheetData>
     <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="19.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="6" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A4" s="4" t="s">
+    <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A18" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A17" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="e" vm="1">
+    <row r="20" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A23" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A39" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A37" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A38" s="4" t="s">
+    <row r="59" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A59" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A60" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A40" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A43" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A45" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" t="e" vm="2">
-        <v>#VALUE!</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="21" x14ac:dyDescent="0.4">
       <c r="A62" s="4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A65" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A67" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A84" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A105" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A107" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A110" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A111" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A83" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A85" s="4" t="s">
+    <row r="130" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A130" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A131" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A154" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A156" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A157" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A88" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A89" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A108" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A109" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A132" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A134" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A135" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A137" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A138" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A140" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A141" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="159" spans="1:1" ht="21" x14ac:dyDescent="0.4">
@@ -1176,49 +1532,149 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A160" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="180" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A180" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="182" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A182" s="4" t="s">
+    <row r="160" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A160" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A162" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A163" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A181" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A202" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A204" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A205" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A208" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A209" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A220" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A237" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A239" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A183" s="1" t="s">
+    <row r="242" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A242" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A243" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A244" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A246" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A185" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="186" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A186" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="188" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A188" s="4" t="s">
+    <row r="259" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A259" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A189" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="200" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A200" s="4" t="s">
+    <row r="275" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A275" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A276" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A278" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A279" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A281" s="4" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A282" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A284" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A297" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A299" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>